<commit_message>
Updated Warrant Modification Spec to match elements used in the Warrant Issued Spec.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26320" yWindow="8040" windowWidth="25600" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="-27300" yWindow="7240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Modification Request " sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="190">
   <si>
     <t>CLASS</t>
   </si>
@@ -339,9 +339,6 @@
     <t>Place Of Birth Code Text</t>
   </si>
   <si>
-    <t>ISO</t>
-  </si>
-  <si>
     <t xml:space="preserve">State ID </t>
   </si>
   <si>
@@ -357,18 +354,9 @@
     <t>scr:</t>
   </si>
   <si>
-    <t>Citizenship Code</t>
-  </si>
-  <si>
-    <t>Ethnicity Code</t>
-  </si>
-  <si>
     <t>Race Code</t>
   </si>
   <si>
-    <t>Sex Code</t>
-  </si>
-  <si>
     <t>SID56567</t>
   </si>
   <si>
@@ -405,12 +393,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Physical Feature Category Code</t>
-  </si>
-  <si>
-    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonPhysicalFeature/j:PhysicalFeatureCategoryCode</t>
-  </si>
-  <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:Case/nc:CaseDocketID</t>
   </si>
   <si>
@@ -441,24 +423,12 @@
     <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonName/nc:PersonFullName</t>
   </si>
   <si>
-    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonCitizenshipISO3166Alpha2Code</t>
-  </si>
-  <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonBirthDate/nc:Date</t>
   </si>
   <si>
-    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonEthnicityCode</t>
-  </si>
-  <si>
-    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonRaceCode</t>
-  </si>
-  <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonEyeColorText</t>
   </si>
   <si>
-    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonSexCode</t>
-  </si>
-  <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:Person/j:PersonAugmentation/j:PersonFBIIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -495,9 +465,6 @@
     <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonRecordIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonAdditionalInformationText</t>
-  </si>
-  <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonCautionCodeText</t>
   </si>
   <si>
@@ -519,9 +486,6 @@
     <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationCityName</t>
   </si>
   <si>
-    <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/j:LocationStateNCICLSTACode</t>
-  </si>
-  <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationPostalCode</t>
   </si>
   <si>
@@ -561,19 +525,70 @@
     <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/scr:TransactionControlNumberIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:WarrantAdditionalInformationText</t>
-  </si>
-  <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonAgeMeasure/nc:MeasureValueText</t>
   </si>
   <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress/nc:LocationStreet/nc:StreetName</t>
   </si>
   <si>
-    <t>Address State Name Code</t>
-  </si>
-  <si>
     <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:WarrantEntryCategoryCodeText</t>
+  </si>
+  <si>
+    <t>Additional Warrant Information Category</t>
+  </si>
+  <si>
+    <t>Person Additional Information Category Text</t>
+  </si>
+  <si>
+    <t>Warrant Additional Information Category</t>
+  </si>
+  <si>
+    <t>Citizenship Text</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonCitizenshipText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonEthnicityText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>Ethnicity Text</t>
+  </si>
+  <si>
+    <t>Sex Text</t>
+  </si>
+  <si>
+    <t>Physical Feature Category Text</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureCategoryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonAdditionalInformation/wm-req-ext:PersonAdditionalInformationCategoryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonAdditionalInformation/wm-req-ext:PersonAdditionalInformationText</t>
+  </si>
+  <si>
+    <t>Person Additional Information Category</t>
+  </si>
+  <si>
+    <t>Address State Name</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStateName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:WarrantAdditionalInformation/wm-req-ext:WarrantAdditionalInformationText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:WarrantAdditionalInformation/wm-req-ext:WarrantAdditionalInformationCategoryText</t>
   </si>
 </sst>
 </file>
@@ -696,9 +711,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="894">
+  <cellStyleXfs count="908">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1643,7 +1672,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="894">
+  <cellStyles count="908">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2090,6 +2119,13 @@
     <cellStyle name="Followed Hyperlink" xfId="889" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="891" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="893" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="895" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="897" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="899" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="901" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="903" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="907" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2536,6 +2572,13 @@
     <cellStyle name="Hyperlink" xfId="888" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="890" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="892" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="894" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="896" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="898" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="900" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="902" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="906" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2871,11 +2914,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F277"/>
+  <dimension ref="A1:F279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2892,7 +2935,7 @@
     <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="6"/>
@@ -2936,7 +2979,7 @@
         <v>66</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="13" customFormat="1">
@@ -2950,10 +2993,10 @@
         <v>67</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="13" customFormat="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="13" customFormat="1" ht="30">
       <c r="A6" s="13" t="s">
         <v>30</v>
       </c>
@@ -2967,10 +3010,10 @@
         <v>68</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="13" customFormat="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="13" customFormat="1" ht="30">
       <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
@@ -2984,7 +3027,7 @@
         <v>69</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="13" customFormat="1" ht="30">
@@ -3001,7 +3044,7 @@
         <v>70</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="13" customFormat="1">
@@ -3025,7 +3068,7 @@
         <v>71</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1">
@@ -3038,7 +3081,7 @@
         <v>72</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="13" customFormat="1">
@@ -3051,7 +3094,7 @@
         <v>73</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="13" customFormat="1">
@@ -3064,7 +3107,7 @@
         <v>74</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="13" customFormat="1">
@@ -3077,7 +3120,7 @@
         <v>75</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1">
@@ -3085,28 +3128,25 @@
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>106</v>
+        <v>174</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>140</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="14" customFormat="1">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E16" s="3">
         <v>24</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="2:6" s="13" customFormat="1">
@@ -3119,31 +3159,31 @@
         <v>23235</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:6" s="13" customFormat="1">
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>113</v>
+        <v>179</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>77</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="2:6" s="13" customFormat="1">
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>83</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="2:6" s="13" customFormat="1">
@@ -3155,22 +3195,22 @@
         <v>78</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="2:6" s="13" customFormat="1">
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>115</v>
+        <v>180</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>84</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" s="13" customFormat="1" ht="30">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" s="13" customFormat="1" ht="45">
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
         <v>14</v>
@@ -3180,20 +3220,20 @@
         <v>354786908</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="2:6" s="13" customFormat="1">
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="2:6" s="13" customFormat="1">
@@ -3205,7 +3245,7 @@
         <v>85</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="2:6" s="13" customFormat="1">
@@ -3217,7 +3257,7 @@
         <v>79</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="2:6" s="13" customFormat="1">
@@ -3230,7 +3270,7 @@
         <v>71</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="2:6" s="13" customFormat="1">
@@ -3243,7 +3283,7 @@
         <v>80</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="2:6" s="13" customFormat="1">
@@ -3256,7 +3296,7 @@
         <v>165</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="2:6" s="13" customFormat="1">
@@ -3269,7 +3309,7 @@
         <v>81</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="2:6" s="13" customFormat="1">
@@ -3281,19 +3321,19 @@
         <v>82</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" s="13" customFormat="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" s="13" customFormat="1" ht="30">
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>128</v>
+        <v>181</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>86</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="2:6" s="13" customFormat="1">
@@ -3306,7 +3346,7 @@
         <v>98213455</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" ht="30">
@@ -3324,10 +3364,10 @@
         <v>90</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="13" customFormat="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="13" customFormat="1" ht="30">
       <c r="A34" s="13" t="s">
         <v>30</v>
       </c>
@@ -3342,308 +3382,308 @@
         <v>91</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="13" customFormat="1">
-      <c r="A35" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="14" customFormat="1" ht="30">
+      <c r="A35" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>51</v>
+        <v>172</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>171</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>89</v>
+        <v>185</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="13" customFormat="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="13" customFormat="1" ht="30">
       <c r="A36" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="13" customFormat="1">
+      <c r="A37" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="B37" s="3" t="s">
+      <c r="F37" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="B38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C38" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3" t="s">
+      <c r="F38" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="13" customFormat="1" ht="30">
-      <c r="B39" s="8" t="s">
+      <c r="F39" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="13" customFormat="1" ht="30">
+      <c r="B40" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="1:6" s="5" customFormat="1" ht="45">
-      <c r="A40" s="5" t="s">
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" s="5" customFormat="1" ht="60">
+      <c r="A41" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="5" customFormat="1" ht="60">
       <c r="B41" s="10"/>
       <c r="C41" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="4">
-        <v>6407</v>
+      <c r="E41" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="5" customFormat="1" ht="45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="5" customFormat="1" ht="60">
       <c r="B42" s="10"/>
       <c r="C42" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4">
+        <v>6407</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="5" customFormat="1" ht="45">
+      <c r="B43" s="10"/>
+      <c r="C43" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4" t="s">
+      <c r="D43" s="4"/>
+      <c r="E43" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="C43" s="4" t="s">
+      <c r="F43" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="C44" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E44" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C44" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>96</v>
-      </c>
       <c r="F44" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="13" customFormat="1" ht="60">
       <c r="C45" s="4" t="s">
-        <v>183</v>
+        <v>25</v>
       </c>
       <c r="E45" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="C46" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C46" s="13" t="s">
+      <c r="F46" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="C47" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E46" s="13">
+      <c r="E47" s="13">
         <v>63412</v>
       </c>
-      <c r="F46" s="13" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="13" customFormat="1">
-      <c r="B47" s="8" t="s">
+      <c r="F47" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="13" customFormat="1">
+      <c r="B48" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-    </row>
-    <row r="48" spans="1:6" s="13" customFormat="1" ht="43" customHeight="1">
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="1:6" s="13" customFormat="1" ht="43" customHeight="1">
+      <c r="C49" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E49" s="13">
         <v>5000</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C49" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="7">
-        <v>40767</v>
-      </c>
       <c r="F49" s="3" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="13" customFormat="1" ht="45">
       <c r="C50" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="7">
+        <v>40767</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C51" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E50" s="13">
+      <c r="E51" s="13">
         <v>659056746</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A51" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E51" s="13" t="b">
-        <v>1</v>
-      </c>
       <c r="F51" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="13" customFormat="1" ht="60">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="13" customFormat="1" ht="45">
       <c r="A52" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="A53" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D53" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E53" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C53" s="3" t="s">
+      <c r="F53" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C54" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D54" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E53" s="13">
+      <c r="E54" s="13">
         <v>758075800</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A54" s="14" t="s">
+      <c r="F54" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A55" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C55" s="13" t="s">
+      <c r="B55" s="14"/>
+      <c r="C55" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C56" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D56" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E56" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="F55" s="13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A56" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="F56" s="13" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3652,98 +3692,131 @@
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E57" s="5">
-        <v>500</v>
+        <v>101</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="13" customFormat="1" ht="45">
       <c r="A58" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>99</v>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58" s="5">
+        <v>500</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="13" customFormat="1" ht="45">
       <c r="A59" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A60" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D59" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A60" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B60" s="15"/>
-      <c r="C60" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>123</v>
+      <c r="E60" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="13" customFormat="1" ht="45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="14" customFormat="1" ht="60">
       <c r="A61" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B61" s="15"/>
       <c r="C61" s="14" t="s">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="13" customFormat="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="A62" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="B62" s="15"/>
-    </row>
-    <row r="63" spans="1:6" s="13" customFormat="1"/>
-    <row r="64" spans="1:6" s="13" customFormat="1"/>
-    <row r="264" hidden="1"/>
-    <row r="265" hidden="1"/>
+      <c r="C62" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A63" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="13" customFormat="1">
+      <c r="B64" s="15"/>
+    </row>
+    <row r="65" s="13" customFormat="1"/>
+    <row r="66" s="13" customFormat="1"/>
     <row r="266" hidden="1"/>
     <row r="267" hidden="1"/>
     <row r="268" hidden="1"/>
@@ -3756,6 +3829,8 @@
     <row r="275" hidden="1"/>
     <row r="276" hidden="1"/>
     <row r="277" hidden="1"/>
+    <row r="278" hidden="1"/>
+    <row r="279" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
Changed "OffenseCodeText" to "GeneralOffenseCharacterDescription Text".
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27300" yWindow="7240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4640" yWindow="3780" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Modification Request " sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>Law Enforcement ORI</t>
   </si>
   <si>
-    <t>Offense Code Text</t>
-  </si>
-  <si>
     <t>Original Offense Code Text</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>Warrant Broadcast Code Text</t>
   </si>
   <si>
-    <t>A code representing an offense</t>
-  </si>
-  <si>
     <t>A code representing an original offense.</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>CN</t>
   </si>
   <si>
-    <t>OC45656-09</t>
-  </si>
-  <si>
     <t>CHG5678</t>
   </si>
   <si>
@@ -399,9 +390,6 @@
     <t>wm-req-doc:WarrantModificationRequest/nc:Case/nc:ActivityIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wm-req-doc:WarrantModificationRequest/nc:Case/j:CaseAugmentation/j:CaseCharge/wm-req-ext:OffenseCodeText</t>
-  </si>
-  <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:Case/j:CaseAugmentation/j:CaseCharge/wm-req-ext:ChargeCodeText</t>
   </si>
   <si>
@@ -589,6 +577,18 @@
   </si>
   <si>
     <t>wm-req-doc:WarrantModificationRequest/j:Warrant[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wm-req-ext:WarrantAugmentation/wm-req-ext:WarrantAdditionalInformation/wm-req-ext:WarrantAdditionalInformationCategoryText</t>
+  </si>
+  <si>
+    <t>General Offense Character Description Text</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Case/j:CaseAugmentation/j:CaseCharge/wm-req-ext:GeneralOffenseCharacterDescriptionText</t>
+  </si>
+  <si>
+    <t>Further description regarding the circumstances of a charge</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -711,9 +711,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="908">
+  <cellStyleXfs count="910">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1672,7 +1674,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="908">
+  <cellStyles count="910">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2126,6 +2128,7 @@
     <cellStyle name="Followed Hyperlink" xfId="903" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="907" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="909" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2579,6 +2582,7 @@
     <cellStyle name="Hyperlink" xfId="902" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="906" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="908" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2916,9 +2920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F279"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2935,7 +2939,7 @@
     <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="6"/>
@@ -2944,7 +2948,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2964,7 +2968,7 @@
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1">
       <c r="B3" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -2976,10 +2980,10 @@
         <v>32</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="13" customFormat="1">
@@ -2990,27 +2994,27 @@
         <v>35</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1" ht="30">
       <c r="A6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>38</v>
+      <c r="C6" s="14" t="s">
+        <v>186</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>68</v>
+        <v>189</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="30">
@@ -3018,16 +3022,16 @@
         <v>30</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="13" customFormat="1" ht="30">
@@ -3035,16 +3039,16 @@
         <v>30</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="13" customFormat="1">
@@ -3065,10 +3069,10 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1">
@@ -3078,10 +3082,10 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="13" customFormat="1">
@@ -3091,10 +3095,10 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="13" customFormat="1">
@@ -3104,10 +3108,10 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="13" customFormat="1">
@@ -3117,10 +3121,10 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1">
@@ -3128,25 +3132,25 @@
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="14" customFormat="1">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E16" s="3">
         <v>24</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="2:6" s="13" customFormat="1">
@@ -3159,55 +3163,55 @@
         <v>23235</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="2:6" s="13" customFormat="1">
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="2:6" s="13" customFormat="1">
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="2:6" s="13" customFormat="1">
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="2:6" s="13" customFormat="1">
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="2:6" s="13" customFormat="1" ht="45">
@@ -3220,44 +3224,44 @@
         <v>354786908</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="2:6" s="13" customFormat="1">
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="2:6" s="13" customFormat="1">
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="2:6" s="13" customFormat="1">
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="2:6" s="13" customFormat="1">
@@ -3270,7 +3274,7 @@
         <v>71</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="2:6" s="13" customFormat="1">
@@ -3280,10 +3284,10 @@
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="2:6" s="13" customFormat="1">
@@ -3296,7 +3300,7 @@
         <v>165</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="2:6" s="13" customFormat="1">
@@ -3306,34 +3310,34 @@
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="2:6" s="13" customFormat="1">
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="2:6" s="13" customFormat="1" ht="30">
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="2:6" s="13" customFormat="1">
@@ -3346,7 +3350,7 @@
         <v>98213455</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" ht="30">
@@ -3355,16 +3359,16 @@
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="13" customFormat="1" ht="30">
@@ -3373,16 +3377,16 @@
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="E34" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="14" customFormat="1" ht="30">
@@ -3391,16 +3395,16 @@
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="13" customFormat="1" ht="30">
@@ -3409,16 +3413,16 @@
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="13" customFormat="1">
@@ -3427,16 +3431,16 @@
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3448,10 +3452,10 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3463,15 +3467,15 @@
         <v>18</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="13" customFormat="1" ht="30">
       <c r="B40" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
@@ -3488,10 +3492,10 @@
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" ht="60">
@@ -3504,7 +3508,7 @@
         <v>6407</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="5" customFormat="1" ht="45">
@@ -3514,10 +3518,10 @@
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="13" customFormat="1" ht="60">
@@ -3525,10 +3529,10 @@
         <v>24</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="13" customFormat="1" ht="60">
@@ -3536,21 +3540,21 @@
         <v>25</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" ht="60">
       <c r="C46" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="13" customFormat="1" ht="60">
@@ -3561,7 +3565,7 @@
         <v>63412</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="13" customFormat="1">
@@ -3575,13 +3579,13 @@
     </row>
     <row r="49" spans="1:6" s="13" customFormat="1" ht="43" customHeight="1">
       <c r="C49" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" s="13">
         <v>5000</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3592,7 +3596,7 @@
         <v>40767</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3603,7 +3607,7 @@
         <v>659056746</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3611,16 +3615,16 @@
         <v>30</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E52" s="13" t="b">
         <v>1</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="13" customFormat="1" ht="60">
@@ -3628,16 +3632,16 @@
         <v>30</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3645,13 +3649,13 @@
         <v>37</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E54" s="13">
         <v>758075800</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3660,30 +3664,30 @@
       </c>
       <c r="B55" s="14"/>
       <c r="C55" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="13" customFormat="1" ht="45">
       <c r="C56" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3692,16 +3696,16 @@
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3710,16 +3714,16 @@
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E58" s="5">
         <v>500</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3727,16 +3731,16 @@
         <v>30</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3744,19 +3748,19 @@
         <v>30</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="14" customFormat="1" ht="60">
@@ -3764,16 +3768,16 @@
         <v>30</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="13" customFormat="1" ht="60">
@@ -3782,16 +3786,16 @@
       </c>
       <c r="B62" s="15"/>
       <c r="C62" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="13" customFormat="1" ht="45">
@@ -3800,16 +3804,16 @@
       </c>
       <c r="B63" s="15"/>
       <c r="C63" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="13" customFormat="1">

</xml_diff>

<commit_message>
Added "PersonUSCitizenIndicator" and "PersonImmigrationAlienQueryIndicator" elements.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="3780" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3460" yWindow="2080" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Modification Request " sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="195">
   <si>
     <t>CLASS</t>
   </si>
@@ -589,6 +589,21 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>US Citizen Indicator</t>
+  </si>
+  <si>
+    <t>PersonImmigationAlienQueryIndicator</t>
+  </si>
+  <si>
+    <t>True if a person query should include the DHS ICE Database; false otherwise.</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/nc:PersonUSCitizenIndicator</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonImmigrationAlienQueryIndicator</t>
   </si>
 </sst>
 </file>
@@ -711,9 +726,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="910">
+  <cellStyleXfs count="912">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1674,7 +1691,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="910">
+  <cellStyles count="912">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2129,6 +2146,7 @@
     <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="907" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="909" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2583,6 +2601,7 @@
     <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="906" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="908" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2918,11 +2937,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F279"/>
+  <dimension ref="A1:F281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3143,268 +3162,262 @@
     </row>
     <row r="16" spans="1:6" s="14" customFormat="1">
       <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="14" customFormat="1" ht="30">
+      <c r="A17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="14" customFormat="1">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E18" s="3">
         <v>24</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="13" customFormat="1">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12">
-        <v>23235</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" s="13" customFormat="1">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" s="13" customFormat="1">
+    <row r="19" spans="1:6" s="13" customFormat="1">
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>80</v>
+        <v>4</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12">
+        <v>23235</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" s="13" customFormat="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="13" customFormat="1">
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>99</v>
+        <v>175</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" s="13" customFormat="1">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="13" customFormat="1">
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>176</v>
+        <v>108</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" s="13" customFormat="1" ht="45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="13" customFormat="1">
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4">
-        <v>354786908</v>
+        <v>99</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" s="13" customFormat="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="13" customFormat="1">
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="4"/>
+        <v>176</v>
+      </c>
       <c r="E23" s="4" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" s="13" customFormat="1">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="13" customFormat="1" ht="45">
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>82</v>
+        <v>14</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4">
+        <v>354786908</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" s="13" customFormat="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="13" customFormat="1">
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>101</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" s="13" customFormat="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="13" customFormat="1">
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4">
-        <v>71</v>
+        <v>100</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" s="13" customFormat="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="13" customFormat="1">
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="4"/>
+        <v>101</v>
+      </c>
       <c r="E27" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" s="13" customFormat="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="13" customFormat="1">
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4">
-        <v>165</v>
+        <v>71</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" s="13" customFormat="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="13" customFormat="1">
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" s="13" customFormat="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="13" customFormat="1">
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>79</v>
+        <v>21</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4">
+        <v>165</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" s="13" customFormat="1" ht="30">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="13" customFormat="1">
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>177</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" s="13" customFormat="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="13" customFormat="1">
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4">
-        <v>98213455</v>
+        <v>102</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" ht="30">
-      <c r="A33" s="13" t="s">
-        <v>30</v>
-      </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>51</v>
+        <v>177</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="13" customFormat="1" ht="30">
-      <c r="A34" s="13" t="s">
-        <v>30</v>
-      </c>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="13" customFormat="1">
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>88</v>
+        <v>6</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4">
+        <v>98213455</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="14" customFormat="1" ht="30">
-      <c r="A35" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="13" customFormat="1" ht="30">
+      <c r="A35" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>167</v>
+        <v>40</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>181</v>
+        <v>87</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>179</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="13" customFormat="1" ht="30">
@@ -3413,416 +3426,450 @@
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="13" customFormat="1">
-      <c r="A37" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="14" customFormat="1" ht="30">
+      <c r="A37" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="13" customFormat="1" ht="30">
+      <c r="A38" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="13" customFormat="1">
+      <c r="A39" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="B38" s="3" t="s">
+    <row r="40" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="B40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C40" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3" t="s">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3" t="s">
+    <row r="41" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="13" customFormat="1" ht="30">
-      <c r="B40" s="8" t="s">
+    <row r="42" spans="1:6" s="13" customFormat="1" ht="30">
+      <c r="B42" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-    </row>
-    <row r="41" spans="1:6" s="5" customFormat="1" ht="60">
-      <c r="A41" s="5" t="s">
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" s="5" customFormat="1" ht="60">
+      <c r="A43" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="5" customFormat="1" ht="60">
-      <c r="B42" s="10"/>
-      <c r="C42" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4">
-        <v>6407</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="5" customFormat="1" ht="45">
       <c r="B43" s="10"/>
       <c r="C43" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="5" customFormat="1" ht="60">
+      <c r="B44" s="10"/>
+      <c r="C44" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4">
+        <v>6407</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="5" customFormat="1" ht="45">
+      <c r="B45" s="10"/>
+      <c r="C45" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="C44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="C45" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" ht="60">
       <c r="C46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="C47" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="C48" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E48" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="C47" s="13" t="s">
+    <row r="49" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="C49" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E47" s="13">
+      <c r="E49" s="13">
         <v>63412</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F49" s="13" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="13" customFormat="1">
-      <c r="B48" s="8" t="s">
+    <row r="50" spans="1:6" s="13" customFormat="1">
+      <c r="B50" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="1:6" s="13" customFormat="1" ht="43" customHeight="1">
-      <c r="C49" s="4" t="s">
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="1:6" s="13" customFormat="1" ht="43" customHeight="1">
+      <c r="C51" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E51" s="13">
         <v>5000</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C50" s="4" t="s">
+    <row r="52" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C52" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E52" s="7">
         <v>40767</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C51" s="4" t="s">
+    <row r="53" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C53" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E53" s="13">
         <v>659056746</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A52" s="13" t="s">
+    <row r="54" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A54" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D54" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="13" t="b">
+      <c r="E54" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="A53" s="13" t="s">
+    <row r="55" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="A55" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D55" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E55" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F55" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C54" s="3" t="s">
+    <row r="56" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C56" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D56" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="13">
+      <c r="E56" s="13">
         <v>758075800</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A55" s="14" t="s">
+    <row r="57" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A57" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="14"/>
-      <c r="C55" s="3" t="s">
+      <c r="B57" s="14"/>
+      <c r="C57" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D57" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E57" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C56" s="13" t="s">
+    <row r="58" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C58" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D58" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E56" s="13" t="s">
+      <c r="E58" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F56" s="13" t="s">
+      <c r="F58" s="13" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A57" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F57" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A58" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E58" s="5">
-        <v>500</v>
-      </c>
-      <c r="F58" s="13" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="13" customFormat="1" ht="45">
       <c r="A59" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C59" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>96</v>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="13" customFormat="1" ht="45">
       <c r="A60" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" s="5">
+        <v>500</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A61" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A62" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C62" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D62" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="E60" s="13" t="s">
+      <c r="E62" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F60" s="14" t="s">
+      <c r="F62" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="14" customFormat="1" ht="60">
-      <c r="A61" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="F61" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="A62" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B62" s="15"/>
-      <c r="C62" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="13" customFormat="1" ht="45">
+    <row r="63" spans="1:6" s="14" customFormat="1" ht="60">
       <c r="A63" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B63" s="15"/>
       <c r="C63" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="A64" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="15"/>
+      <c r="C64" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A65" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" s="15"/>
+      <c r="C65" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D65" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E65" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="F63" s="14" t="s">
+      <c r="F65" s="14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="13" customFormat="1">
-      <c r="B64" s="15"/>
-    </row>
-    <row r="65" s="13" customFormat="1"/>
-    <row r="66" s="13" customFormat="1"/>
-    <row r="266" hidden="1"/>
-    <row r="267" hidden="1"/>
+    <row r="66" spans="1:6" s="13" customFormat="1">
+      <c r="B66" s="15"/>
+    </row>
+    <row r="67" spans="1:6" s="13" customFormat="1"/>
+    <row r="68" spans="1:6" s="13" customFormat="1"/>
     <row r="268" hidden="1"/>
     <row r="269" hidden="1"/>
     <row r="270" hidden="1"/>
@@ -3835,6 +3882,8 @@
     <row r="277" hidden="1"/>
     <row r="278" hidden="1"/>
     <row r="279" hidden="1"/>
+    <row r="280" hidden="1"/>
+    <row r="281" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
Added vehcile/conveyance elements and associations to the Warrant Modification Request IEPD.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="2080" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2260" yWindow="2620" windowWidth="30320" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Modification Request " sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="233">
   <si>
     <t>CLASS</t>
   </si>
@@ -604,6 +604,120 @@
   </si>
   <si>
     <t>wm-req-doc:WarrantModificationRequest/nc:Person/wm-req-ext:PersonImmigrationAlienQueryIndicator</t>
+  </si>
+  <si>
+    <t>VEHICLE</t>
+  </si>
+  <si>
+    <t>License Plate Number</t>
+  </si>
+  <si>
+    <t>LP4365-0234</t>
+  </si>
+  <si>
+    <t>License Plate Category Text</t>
+  </si>
+  <si>
+    <t>LP-category</t>
+  </si>
+  <si>
+    <t>Vehicle Registration Expiration Date</t>
+  </si>
+  <si>
+    <t>2016-11</t>
+  </si>
+  <si>
+    <t>Vehicle Primary Color Code Text</t>
+  </si>
+  <si>
+    <t>BGE</t>
+  </si>
+  <si>
+    <t>Vehicle Secondary Color Code Text</t>
+  </si>
+  <si>
+    <t>BRO</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>VIN3458745679777</t>
+  </si>
+  <si>
+    <t>Vehicle Make Name</t>
+  </si>
+  <si>
+    <t>NCIC</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>Vehicle Model Name</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>Vehicle Style Text</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>Vehicle Year</t>
+  </si>
+  <si>
+    <t>Additional Vehicle Information Category Text</t>
+  </si>
+  <si>
+    <t>Vehicle Information Category</t>
+  </si>
+  <si>
+    <t>Additional Vehicle Information Text</t>
+  </si>
+  <si>
+    <t>Additional information about a vehicle.</t>
+  </si>
+  <si>
+    <t>Excessive Rust</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistration[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistration[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:ConveyanceRegistrationPlateCategoryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistration[@structures:id=/wm-req-doc:WarrantModificationRequest/j:ConveyanceRegistrationAssociation/j:ItemRegistration/@structures:ref]/j:RegistrationExpirationDate/nc:YearMonthDate</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorPrimaryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorSecondaryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemMakeName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemModelName</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemStyleText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemModelYearDate</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wm-req-ext:VehicleAdditionalInformation/wm-req-ext:VehicleAdditionalInformationCategoryText</t>
+  </si>
+  <si>
+    <t>wm-req-doc:WarrantModificationRequest/nc:Vehicle[@structures:id=/wm-req-doc:WarrantModificationRequest/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wm-req-ext:VehicleAdditionalInformation/wm-req-ext:VehicleAdditionalInformationText</t>
   </si>
 </sst>
 </file>
@@ -2937,11 +3051,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F281"/>
+  <dimension ref="A1:F294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD17"/>
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3507,7 +3621,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="13" customFormat="1" ht="45">
+    <row r="41" spans="1:6" s="14" customFormat="1" ht="45">
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
         <v>17</v>
@@ -3522,368 +3636,528 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="13" customFormat="1" ht="30">
+    <row r="42" spans="1:6" s="14" customFormat="1">
       <c r="B42" s="8" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="1:6" s="5" customFormat="1" ht="60">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="C43" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="C44" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="14" customFormat="1" ht="56" customHeight="1">
+      <c r="C45" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="C46" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="C47" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="C48" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="C49" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="C50" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="14" customFormat="1" ht="45" customHeight="1">
+      <c r="C51" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="C52" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E52" s="14">
+        <v>2012</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="A53" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="4" t="s">
+      <c r="C53" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="14" customFormat="1" ht="45">
+      <c r="A54" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="14" customFormat="1" ht="30">
+      <c r="B55" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="1:6" s="5" customFormat="1" ht="60">
+      <c r="A56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4" t="s">
+      <c r="D56" s="4"/>
+      <c r="E56" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="5" customFormat="1" ht="60">
-      <c r="B44" s="10"/>
-      <c r="C44" s="4" t="s">
+    <row r="57" spans="1:6" s="5" customFormat="1" ht="60">
+      <c r="B57" s="10"/>
+      <c r="C57" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4">
+      <c r="D57" s="4"/>
+      <c r="E57" s="4">
         <v>6407</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="5" customFormat="1" ht="45">
-      <c r="B45" s="10"/>
-      <c r="C45" s="4" t="s">
+    <row r="58" spans="1:6" s="5" customFormat="1" ht="45">
+      <c r="B58" s="10"/>
+      <c r="C58" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4" t="s">
+      <c r="D58" s="4"/>
+      <c r="E58" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F58" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="C46" s="4" t="s">
+    <row r="59" spans="1:6" s="14" customFormat="1" ht="60">
+      <c r="C59" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E59" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F59" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="C47" s="4" t="s">
+    <row r="60" spans="1:6" s="14" customFormat="1" ht="60">
+      <c r="C60" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E60" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F60" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="C48" s="4" t="s">
+    <row r="61" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="C61" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E61" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="C49" s="13" t="s">
+    <row r="62" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="C62" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E62" s="13">
         <v>63412</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F62" s="13" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="13" customFormat="1">
-      <c r="B50" s="8" t="s">
+    <row r="63" spans="1:6" s="13" customFormat="1">
+      <c r="B63" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-    </row>
-    <row r="51" spans="1:6" s="13" customFormat="1" ht="43" customHeight="1">
-      <c r="C51" s="4" t="s">
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="1:6" s="13" customFormat="1" ht="43" customHeight="1">
+      <c r="C64" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E64" s="13">
         <v>5000</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F64" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C52" s="4" t="s">
+    <row r="65" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C65" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E65" s="7">
         <v>40767</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F65" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C53" s="4" t="s">
+    <row r="66" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C66" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E53" s="13">
+      <c r="E66" s="13">
         <v>659056746</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F66" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A54" s="13" t="s">
+    <row r="67" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A67" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D67" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="13" t="b">
+      <c r="E67" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="F67" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="A55" s="13" t="s">
+    <row r="68" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="A68" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D68" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E68" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F68" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C56" s="3" t="s">
+    <row r="69" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C69" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D69" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E56" s="13">
+      <c r="E69" s="13">
         <v>758075800</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F69" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A57" s="14" t="s">
+    <row r="70" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A70" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="3" t="s">
+      <c r="B70" s="14"/>
+      <c r="C70" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D70" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E57" s="13" t="s">
+      <c r="E70" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F70" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="C58" s="13" t="s">
+    <row r="71" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="C71" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D71" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E71" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F58" s="13" t="s">
+      <c r="F71" s="13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A59" s="13" t="s">
+    <row r="72" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A72" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5" t="s">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D72" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E72" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F72" s="13" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A60" s="13" t="s">
+    <row r="73" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A73" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5" t="s">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D73" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E60" s="5">
+      <c r="E73" s="5">
         <v>500</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F73" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A61" s="13" t="s">
+    <row r="74" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A74" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C74" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D74" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E74" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F61" s="13" t="s">
+      <c r="F74" s="13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A62" s="13" t="s">
+    <row r="75" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A75" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B75" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C75" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D75" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="E62" s="13" t="s">
+      <c r="E75" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F62" s="14" t="s">
+      <c r="F75" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="14" customFormat="1" ht="60">
-      <c r="A63" s="14" t="s">
+    <row r="76" spans="1:6" s="14" customFormat="1" ht="60">
+      <c r="A76" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C76" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D76" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E76" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="F63" s="14" t="s">
+      <c r="F76" s="14" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="13" customFormat="1" ht="60">
-      <c r="A64" s="14" t="s">
+    <row r="77" spans="1:6" s="13" customFormat="1" ht="60">
+      <c r="A77" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="15"/>
-      <c r="C64" s="14" t="s">
+      <c r="B77" s="15"/>
+      <c r="C77" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D77" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E77" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="F64" s="14" t="s">
+      <c r="F77" s="14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="13" customFormat="1" ht="45">
-      <c r="A65" s="14" t="s">
+    <row r="78" spans="1:6" s="13" customFormat="1" ht="45">
+      <c r="A78" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B65" s="15"/>
-      <c r="C65" s="14" t="s">
+      <c r="B78" s="15"/>
+      <c r="C78" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D65" s="14" t="s">
+      <c r="D78" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E78" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="F65" s="14" t="s">
+      <c r="F78" s="14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="13" customFormat="1">
-      <c r="B66" s="15"/>
-    </row>
-    <row r="67" spans="1:6" s="13" customFormat="1"/>
-    <row r="68" spans="1:6" s="13" customFormat="1"/>
-    <row r="268" hidden="1"/>
-    <row r="269" hidden="1"/>
-    <row r="270" hidden="1"/>
-    <row r="271" hidden="1"/>
-    <row r="272" hidden="1"/>
-    <row r="273" hidden="1"/>
-    <row r="274" hidden="1"/>
-    <row r="275" hidden="1"/>
-    <row r="276" hidden="1"/>
-    <row r="277" hidden="1"/>
-    <row r="278" hidden="1"/>
-    <row r="279" hidden="1"/>
-    <row r="280" hidden="1"/>
+    <row r="79" spans="1:6" s="13" customFormat="1">
+      <c r="B79" s="15"/>
+    </row>
+    <row r="80" spans="1:6" s="13" customFormat="1"/>
+    <row r="81" s="13" customFormat="1"/>
     <row r="281" hidden="1"/>
+    <row r="282" hidden="1"/>
+    <row r="283" hidden="1"/>
+    <row r="284" hidden="1"/>
+    <row r="285" hidden="1"/>
+    <row r="286" hidden="1"/>
+    <row r="287" hidden="1"/>
+    <row r="288" hidden="1"/>
+    <row r="289" hidden="1"/>
+    <row r="290" hidden="1"/>
+    <row r="291" hidden="1"/>
+    <row r="292" hidden="1"/>
+    <row r="293" hidden="1"/>
+    <row r="294" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
Updated LE ORI in sample message.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Modification_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1740" windowWidth="26360" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="4080" yWindow="1740" windowWidth="26355" windowHeight="16275" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Modification Request " sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="226">
   <si>
     <t>CLASS</t>
   </si>
@@ -195,12 +195,6 @@
     <t>CN</t>
   </si>
   <si>
-    <t>CHG5678</t>
-  </si>
-  <si>
-    <t>OO4356788</t>
-  </si>
-  <si>
     <t>Peter</t>
   </si>
   <si>
@@ -489,9 +483,6 @@
     <t>Further description regarding the circumstances of a charge</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>US Citizen Indicator</t>
   </si>
   <si>
@@ -703,6 +694,9 @@
   </si>
   <si>
     <t>Extradition Limit Code Text</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -3022,35 +3016,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="11" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="32.875" style="11" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="92.33203125" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="28.375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="92.375" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23" customHeight="1">
+    <row r="1" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>0</v>
@@ -3068,7 +3062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>52</v>
       </c>
@@ -3077,7 +3071,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
@@ -3085,10 +3079,10 @@
         <v>56</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
@@ -3099,27 +3093,27 @@
         <v>57</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>156</v>
+        <v>225</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>27</v>
       </c>
@@ -3129,14 +3123,14 @@
       <c r="D7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>58</v>
+      <c r="E7" s="11">
+        <v>4901</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>27</v>
       </c>
@@ -3146,49 +3140,49 @@
       <c r="D8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>59</v>
+      <c r="E8" s="11">
+        <v>750.11500000000001</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
@@ -3197,7 +3191,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -3206,122 +3200,122 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E18" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
         <v>4</v>
@@ -3331,58 +3325,58 @@
         <v>23235</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
         <v>14</v>
@@ -3392,47 +3386,47 @@
         <v>354786908</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
         <v>19</v>
@@ -3442,23 +3436,23 @@
         <v>71</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
         <v>21</v>
@@ -3468,47 +3462,47 @@
         <v>165</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
         <v>6</v>
@@ -3518,10 +3512,10 @@
         <v>98213455</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>27</v>
       </c>
@@ -3533,13 +3527,13 @@
         <v>44</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>27</v>
       </c>
@@ -3551,13 +3545,13 @@
         <v>43</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>15</v>
       </c>
@@ -3566,13 +3560,13 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
         <v>17</v>
@@ -3581,166 +3575,166 @@
         <v>18</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="1:6" ht="45">
+    <row r="42" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C43" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="F43" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="45">
-      <c r="C43" s="2" t="s">
+      <c r="E44" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="56" customHeight="1">
-      <c r="C44" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>168</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="56" customHeight="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E45" s="11" t="b">
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="56" customHeight="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C47" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C48" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="F48" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C49" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="E49" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C50" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="45">
-      <c r="C48" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="F48" s="1" t="s">
+    <row r="51" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C51" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="45">
-      <c r="C49" s="2" t="s">
+    <row r="52" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E49" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="F49" s="1" t="s">
+      <c r="E52" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="45">
-      <c r="C50" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="45">
-      <c r="C51" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E51" s="11" t="s">
+    <row r="53" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C53" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="45" customHeight="1">
-      <c r="C52" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="45">
-      <c r="C53" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E53" s="11">
         <v>2012</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="30">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>38</v>
       </c>
@@ -3749,7 +3743,7 @@
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" ht="60">
+    <row r="55" spans="1:6" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>27</v>
       </c>
@@ -3759,48 +3753,48 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" ht="60">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="B56" s="8"/>
       <c r="C56" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="60">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="60">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="60">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="C59" s="11" t="s">
         <v>26</v>
       </c>
@@ -3808,10 +3802,10 @@
         <v>63412</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
         <v>28</v>
       </c>
@@ -3820,21 +3814,21 @@
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" ht="45">
+    <row r="61" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C61" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E61" s="5">
         <v>41133</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="43" customHeight="1">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="2" t="s">
         <v>42</v>
       </c>
@@ -3842,10 +3836,10 @@
         <v>5000</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C63" s="2" t="s">
         <v>33</v>
       </c>
@@ -3853,10 +3847,10 @@
         <v>40767</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C64" s="2" t="s">
         <v>30</v>
       </c>
@@ -3864,21 +3858,21 @@
         <v>659056746</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C65" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>27</v>
       </c>
@@ -3892,27 +3886,27 @@
         <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="60">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C68" s="1" t="s">
         <v>34</v>
       </c>
@@ -3923,27 +3917,27 @@
         <v>758075800</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D69" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="E69" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C70" s="11" t="s">
         <v>55</v>
       </c>
@@ -3951,13 +3945,13 @@
         <v>41</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>27</v>
       </c>
@@ -3972,10 +3966,10 @@
         <v>500</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>27</v>
       </c>
@@ -3986,94 +3980,94 @@
         <v>39</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C74" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F74" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="D74" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="45">
+    </row>
+    <row r="75" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C75" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E75" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D75" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>101</v>
-      </c>
       <c r="F75" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D76" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F76" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="E76" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="278" hidden="1"/>
-    <row r="279" hidden="1"/>
-    <row r="280" hidden="1"/>
-    <row r="281" hidden="1"/>
-    <row r="282" hidden="1"/>
-    <row r="283" hidden="1"/>
-    <row r="284" hidden="1"/>
-    <row r="285" hidden="1"/>
-    <row r="286" hidden="1"/>
-    <row r="287" hidden="1"/>
-    <row r="288" hidden="1"/>
-    <row r="289" hidden="1"/>
-    <row r="290" hidden="1"/>
-    <row r="291" hidden="1"/>
+    </row>
+    <row r="278" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>

</xml_diff>